<commit_message>
Reset to clean things not needed
</commit_message>
<xml_diff>
--- a/FAERS ID_AE/Delinquency.xlsx
+++ b/FAERS ID_AE/Delinquency.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="206">
   <si>
     <t>Case ID</t>
   </si>
@@ -97,180 +97,180 @@
     <t>Product Used For Unknown Indication;Schizophrenia</t>
   </si>
   <si>
-    <t>Delinquency;Aggression;Boredom;Hospitalisation</t>
+    <t>Boredom;Hospitalisation;Aggression;Delinquency</t>
+  </si>
+  <si>
+    <t>Hospitalized;Other Outcomes</t>
+  </si>
+  <si>
+    <t>Not Specified</t>
+  </si>
+  <si>
+    <t>29-MAR-2018</t>
+  </si>
+  <si>
+    <t>Expedited</t>
+  </si>
+  <si>
+    <t>Cipla</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Lyrica</t>
+  </si>
+  <si>
+    <t>14-MAR-2018</t>
+  </si>
+  <si>
+    <t>12-JAN-2018</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DE-CIPLA LTD.-2018DE00172</t>
+  </si>
+  <si>
+    <t>Risperdal;Risperdal Consta</t>
+  </si>
+  <si>
+    <t>Risperidone;Risperidone</t>
+  </si>
+  <si>
+    <t>Schizophrenia</t>
+  </si>
+  <si>
+    <t>Delinquency;Boredom;Aggression;Hospitalisation</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>06-MAR-2018</t>
+  </si>
+  <si>
+    <t>42 YR</t>
+  </si>
+  <si>
+    <t>114 KG</t>
+  </si>
+  <si>
+    <t>Janssen</t>
+  </si>
+  <si>
+    <t>27-FEB-2018</t>
+  </si>
+  <si>
+    <t>27-NOV-2017</t>
+  </si>
+  <si>
+    <t>DE-JNJFOC-20171120513</t>
+  </si>
+  <si>
+    <t>Lorazepam</t>
+  </si>
+  <si>
+    <t>Crime;Delinquency;Aggression;Anger;Imprisonment;Impulsive Behaviour;Drug Withdrawal Syndrome;Libido Decreased;Alcohol Use</t>
+  </si>
+  <si>
+    <t>Hospitalized</t>
+  </si>
+  <si>
+    <t>1990</t>
+  </si>
+  <si>
+    <t>28-MAY-2015</t>
+  </si>
+  <si>
+    <t>Amneal</t>
+  </si>
+  <si>
+    <t>Clorazepate Dipotassium;Paxil</t>
+  </si>
+  <si>
+    <t>12-MAY-2015</t>
+  </si>
+  <si>
+    <t>BB15-136-AE</t>
+  </si>
+  <si>
+    <t>Abilify</t>
+  </si>
+  <si>
+    <t>Aripiprazole</t>
+  </si>
+  <si>
+    <t>Anger;Delinquency</t>
+  </si>
+  <si>
+    <t>Other Outcomes</t>
+  </si>
+  <si>
+    <t>16-DEC-2011</t>
+  </si>
+  <si>
+    <t>Non-Expedited</t>
+  </si>
+  <si>
+    <t>2 DEC</t>
+  </si>
+  <si>
+    <t>Bristol Myers Squibb</t>
+  </si>
+  <si>
+    <t>21-MAR-2011</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>US-BRISTOL-MYERS SQUIBB COMPANY-15621311</t>
+  </si>
+  <si>
+    <t>Pristiq Extended-Release</t>
+  </si>
+  <si>
+    <t>Desvenlafaxine Succinate</t>
+  </si>
+  <si>
+    <t>Anxiety</t>
+  </si>
+  <si>
+    <t>Aggression;Suicide Attempt;Mania;Delinquency;Abnormal Behaviour;Post-Traumatic Stress Disorder;Drug Effect Decreased</t>
+  </si>
+  <si>
+    <t>08-OCT-2010</t>
+  </si>
+  <si>
+    <t>Wyeth</t>
+  </si>
+  <si>
+    <t>28-SEP-2010</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>AU-WYE-G06736910</t>
+  </si>
+  <si>
+    <t>Strattera</t>
+  </si>
+  <si>
+    <t>Atomoxetine Hydrochloride</t>
+  </si>
+  <si>
+    <t>Attention Deficit/Hyperactivity Disorder;Hypertension</t>
+  </si>
+  <si>
+    <t>Delinquency;Depression;Heart Rate Increased;Intentional Self-Injury;Personality Change;Suicide Attempt;Hand Fracture;Aggression;Hostility;Hypertension</t>
   </si>
   <si>
     <t>Other Outcomes;Hospitalized</t>
   </si>
   <si>
-    <t>Not Specified</t>
-  </si>
-  <si>
-    <t>29-MAR-2018</t>
-  </si>
-  <si>
-    <t>Expedited</t>
-  </si>
-  <si>
-    <t>Cipla</t>
-  </si>
-  <si>
-    <t>Consumer</t>
-  </si>
-  <si>
-    <t>Lyrica</t>
-  </si>
-  <si>
-    <t>14-MAR-2018</t>
-  </si>
-  <si>
-    <t>12-JAN-2018</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>DE-CIPLA LTD.-2018DE00172</t>
-  </si>
-  <si>
-    <t>Risperdal;Risperdal Consta</t>
-  </si>
-  <si>
-    <t>Risperidone;Risperidone</t>
-  </si>
-  <si>
-    <t>Schizophrenia</t>
-  </si>
-  <si>
-    <t>Hospitalisation;Boredom;Aggression;Delinquency</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>06-MAR-2018</t>
-  </si>
-  <si>
-    <t>42 YR</t>
-  </si>
-  <si>
-    <t>114 KG</t>
-  </si>
-  <si>
-    <t>Janssen</t>
-  </si>
-  <si>
-    <t>27-FEB-2018</t>
-  </si>
-  <si>
-    <t>27-NOV-2017</t>
-  </si>
-  <si>
-    <t>DE-JNJFOC-20171120513</t>
-  </si>
-  <si>
-    <t>Lorazepam</t>
-  </si>
-  <si>
-    <t>Aggression;Drug Withdrawal Syndrome;Alcohol Use;Crime;Impulsive Behaviour;Anger;Imprisonment;Libido Decreased;Delinquency</t>
-  </si>
-  <si>
-    <t>Hospitalized</t>
-  </si>
-  <si>
-    <t>1990</t>
-  </si>
-  <si>
-    <t>28-MAY-2015</t>
-  </si>
-  <si>
-    <t>Amneal</t>
-  </si>
-  <si>
-    <t>Clorazepate Dipotassium;Paxil</t>
-  </si>
-  <si>
-    <t>12-MAY-2015</t>
-  </si>
-  <si>
-    <t>BB15-136-AE</t>
-  </si>
-  <si>
-    <t>Abilify</t>
-  </si>
-  <si>
-    <t>Aripiprazole</t>
-  </si>
-  <si>
-    <t>Delinquency;Anger</t>
-  </si>
-  <si>
-    <t>Other Outcomes</t>
-  </si>
-  <si>
-    <t>16-DEC-2011</t>
-  </si>
-  <si>
-    <t>Non-Expedited</t>
-  </si>
-  <si>
-    <t>2 DEC</t>
-  </si>
-  <si>
-    <t>Bristol Myers Squibb</t>
-  </si>
-  <si>
-    <t>21-MAR-2011</t>
-  </si>
-  <si>
-    <t>US</t>
-  </si>
-  <si>
-    <t>US-BRISTOL-MYERS SQUIBB COMPANY-15621311</t>
-  </si>
-  <si>
-    <t>Pristiq Extended-Release</t>
-  </si>
-  <si>
-    <t>Desvenlafaxine Succinate</t>
-  </si>
-  <si>
-    <t>Anxiety</t>
-  </si>
-  <si>
-    <t>Delinquency;Aggression;Drug Effect Decreased;Suicide Attempt;Mania;Abnormal Behaviour;Post-Traumatic Stress Disorder</t>
-  </si>
-  <si>
-    <t>Hospitalized;Other Outcomes</t>
-  </si>
-  <si>
-    <t>08-OCT-2010</t>
-  </si>
-  <si>
-    <t>Wyeth</t>
-  </si>
-  <si>
-    <t>28-SEP-2010</t>
-  </si>
-  <si>
-    <t>AU</t>
-  </si>
-  <si>
-    <t>AU-WYE-G06736910</t>
-  </si>
-  <si>
-    <t>Strattera</t>
-  </si>
-  <si>
-    <t>Atomoxetine Hydrochloride</t>
-  </si>
-  <si>
-    <t>Attention Deficit/Hyperactivity Disorder;Hypertension</t>
-  </si>
-  <si>
-    <t>Hand Fracture;Personality Change;Heart Rate Increased;Suicide Attempt;Intentional Self-Injury;Depression;Hypertension;Delinquency;Aggression;Hostility</t>
-  </si>
-  <si>
     <t>01-JAN-2008</t>
   </si>
   <si>
@@ -307,7 +307,7 @@
     <t>Venlafaxine Hydrochloride;Alcohol</t>
   </si>
   <si>
-    <t>Hallucination, Auditory;Alcohol Interaction;Antisocial Behaviour;Delinquency;Fatigue</t>
+    <t>Hallucination, Auditory;Fatigue;Delinquency;Alcohol Interaction;Antisocial Behaviour</t>
   </si>
   <si>
     <t>Female</t>
@@ -337,10 +337,10 @@
     <t>Seasonal Allergy</t>
   </si>
   <si>
-    <t>Alcohol Use;Educational Problem;Suicidal Ideation;Delinquency;Abnormal Behaviour;Drug Abuse</t>
-  </si>
-  <si>
-    <t>Other Outcomes;Required Intervention</t>
+    <t>Educational Problem;Abnormal Behaviour;Alcohol Use;Drug Abuse;Delinquency;Suicidal Ideation</t>
+  </si>
+  <si>
+    <t>Required Intervention;Other Outcomes</t>
   </si>
   <si>
     <t>23-APR-2008</t>
@@ -391,7 +391,7 @@
     <t>Product Used For Unknown Indication</t>
   </si>
   <si>
-    <t>Schizophrenia;Delinquency</t>
+    <t>Delinquency;Schizophrenia</t>
   </si>
   <si>
     <t>24-AUG-2007</t>
@@ -406,10 +406,13 @@
     <t>US-ROCHE-511718</t>
   </si>
   <si>
+    <t>Risperdal Consta;Risperdal</t>
+  </si>
+  <si>
     <t>Depression;Poor Quality Sleep;Product Used For Unknown Indication;Schizophrenia</t>
   </si>
   <si>
-    <t>Overdose;Schizophrenia;Delinquency;Depression</t>
+    <t>Overdose;Schizophrenia;Depression;Delinquency</t>
   </si>
   <si>
     <t>29-MAR-2006</t>
@@ -439,7 +442,7 @@
     <t>Disturbance In Attention</t>
   </si>
   <si>
-    <t>Social Avoidant Behaviour;Mood Altered;Aggression;Anger;Delinquency;Condition Aggravated;Depression</t>
+    <t>Delinquency;Mood Altered;Depression;Condition Aggravated;Anger;Aggression;Social Avoidant Behaviour</t>
   </si>
   <si>
     <t>OCT-2005</t>
@@ -466,7 +469,7 @@
     <t>Micturition Urgency;Parkinson'S Disease;Tremor</t>
   </si>
   <si>
-    <t>Delinquency;Gambling Disorder;Treatment Noncompliance;Suicide Attempt;Personality Disorder</t>
+    <t>Treatment Noncompliance;Suicide Attempt;Delinquency;Personality Disorder;Gambling Disorder</t>
   </si>
   <si>
     <t>01-JAN-2004</t>
@@ -478,7 +481,7 @@
     <t>Boehringer Ingelheim</t>
   </si>
   <si>
-    <t>Selegiline Hydrochloride;Detrol</t>
+    <t>Detrol;Selegiline Hydrochloride</t>
   </si>
   <si>
     <t>19-OCT-2005</t>
@@ -490,16 +493,16 @@
     <t>Oxycontin</t>
   </si>
   <si>
-    <t>Oxycodone Hydrochloride;Cannabis Sativa Subsp. Sativa Flowering Top;Amitriptyline Hydrochloride;Acetaminophen\Hydrocodone Bitartrate;Acetaminophen</t>
+    <t>Oxycodone Hydrochloride;Amitriptyline Hydrochloride;Acetaminophen;Cannabis Sativa Subsp. Sativa Flowering Top;Acetaminophen\Hydrocodone Bitartrate</t>
   </si>
   <si>
     <t>Pain</t>
   </si>
   <si>
-    <t>Drug Withdrawal Syndrome;Dyspepsia;Chronic Obstructive Pulmonary Disease;Arthralgia;Alcoholism;Speech Disorder;Somnolence;Depressed Level Of Consciousness;Learning Disability;Delirium;Cardiomegaly;Hand Fracture;Pain In Extremity;Overdose;Male Sexual Dysfunction;Musculoskeletal Stiffness;Obesity;Delinquency;Tooth Extraction;Asthenia;Major Depression;Pollakiuria;Bronchitis;Abnormal Behaviour;Drug Abuser;Fall;Diarrhoea;Generalised Anxiety Disorder;Paraesthesia;Pyrexia;Anxiety;Bone Pain;Toxicity To Various Agents;Hypertension;Spinal Osteoarthritis;Hypoaesthesia;Vomiting;Pneumoconiosis;Nocturia;Emotional Distress;Borderline Mental Impairment;Urinary Incontinence;Suicidal Ideation;Drug Dependence;Inadequate Analgesia</t>
-  </si>
-  <si>
-    <t>Hospitalized;Died;Other Outcomes</t>
+    <t>Alcoholism;Spinal Osteoarthritis;Learning Disability;Male Sexual Dysfunction;Bronchitis;Vomiting;Borderline Mental Impairment;Fall;Delirium;Pollakiuria;Somnolence;Pyrexia;Hand Fracture;Obesity;Pneumoconiosis;Hypertension;Urinary Incontinence;Nocturia;Overdose;Paraesthesia;Asthenia;Inadequate Analgesia;Depressed Level Of Consciousness;Diarrhoea;Generalised Anxiety Disorder;Emotional Distress;Major Depression;Cardiomegaly;Drug Dependence;Bone Pain;Chronic Obstructive Pulmonary Disease;Arthralgia;Toxicity To Various Agents;Hypoaesthesia;Delinquency;Musculoskeletal Stiffness;Speech Disorder;Dyspepsia;Suicidal Ideation;Drug Withdrawal Syndrome;Abnormal Behaviour;Pain In Extremity;Tooth Extraction;Anxiety;Drug Abuser</t>
+  </si>
+  <si>
+    <t>Other Outcomes;Died;Hospitalized</t>
   </si>
   <si>
     <t>21-OCT-1998</t>
@@ -520,7 +523,7 @@
     <t>Consumer,Health Professional</t>
   </si>
   <si>
-    <t>Diazepam;Vioxx;Pamelor;Lorcet;Ambien;Ativan;Prednisone;Cogentin;Theo-Dur;Haldol;Buspar;Soma;Tenormin;Xanax;Skelaxin;Phenergan;Percocet;Baclofen;Ultram;Narcan;Toradol;Flovent</t>
+    <t>Theo-Dur;Phenergan;Lorcet;Ultram;Ambien;Narcan;Flovent;Cogentin;Percocet;Xanax;Haldol;Vioxx;Skelaxin;Buspar;Soma;Baclofen;Pamelor;Tenormin;Toradol;Prednisone;Diazepam;Ativan</t>
   </si>
   <si>
     <t>24-MAY-2005</t>
@@ -538,7 +541,7 @@
     <t>Attention Deficit/Hyperactivity Disorder</t>
   </si>
   <si>
-    <t>Abnormal Behaviour;Theft;Delinquency</t>
+    <t>Theft;Abnormal Behaviour;Delinquency</t>
   </si>
   <si>
     <t>30-JUL-2002</t>
@@ -559,7 +562,7 @@
     <t>Depression</t>
   </si>
   <si>
-    <t>Theft;Legal Problem;Personality Change;Pyromania;Physical Assault;Thinking Abnormal;Delinquency</t>
+    <t>Theft;Thinking Abnormal;Legal Problem;Personality Change;Delinquency;Pyromania;Physical Assault</t>
   </si>
   <si>
     <t>08-APR-2002</t>
@@ -589,7 +592,7 @@
     <t>Sertraline Hydrochloride;Bupropion Hydrochloride</t>
   </si>
   <si>
-    <t>Drug Abuser;Obsessive-Compulsive Disorder;Delinquency;Alcoholism;Suicide Attempt;Imprisonment;Abnormal Behaviour;Paraphilia;Theft;Thinking Abnormal</t>
+    <t>Thinking Abnormal;Paraphilia;Drug Abuser;Theft;Abnormal Behaviour;Obsessive-Compulsive Disorder;Delinquency;Alcoholism;Suicide Attempt;Imprisonment</t>
   </si>
   <si>
     <t>Life Threatening;Disabled</t>
@@ -613,7 +616,7 @@
     <t>Fluoxetine Hydrochloride</t>
   </si>
   <si>
-    <t>Thinking Abnormal;Aggression;Physical Assault;Suicidal Ideation;Imprisonment;Depressed Mood;Delinquency;Anxiety</t>
+    <t>Depressed Mood;Suicidal Ideation;Physical Assault;Imprisonment;Delinquency;Aggression;Anxiety;Thinking Abnormal</t>
   </si>
   <si>
     <t>OCT-1991</t>
@@ -1386,7 +1389,7 @@
         <v>5</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>28</v>
       </c>
       <c r="H6" t="s">
         <v>43</v>
@@ -1395,7 +1398,7 @@
         <v>24</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K6" t="s">
         <v>31</v>
@@ -1407,7 +1410,7 @@
         <v>29</v>
       </c>
       <c r="N6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O6" t="s">
         <v>33</v>
@@ -1419,19 +1422,19 @@
         <v>24</v>
       </c>
       <c r="R6" t="s">
+        <v>77</v>
+      </c>
+      <c r="S6" t="s">
+        <v>75</v>
+      </c>
+      <c r="T6" t="s">
         <v>78</v>
       </c>
-      <c r="S6" t="s">
-        <v>76</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
+        <v>29</v>
+      </c>
+      <c r="V6" t="s">
         <v>79</v>
-      </c>
-      <c r="U6" t="s">
-        <v>29</v>
-      </c>
-      <c r="V6" t="s">
-        <v>80</v>
       </c>
       <c r="W6" t="s">
         <v>24</v>
@@ -1445,22 +1448,22 @@
         <v>7041833</v>
       </c>
       <c r="B7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" t="s">
         <v>81</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>82</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>83</v>
-      </c>
-      <c r="E7" t="s">
-        <v>84</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>28</v>
+        <v>84</v>
       </c>
       <c r="H7" t="s">
         <v>43</v>
@@ -1555,7 +1558,7 @@
         <v>29</v>
       </c>
       <c r="N8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O8" t="s">
         <v>33</v>
@@ -1815,16 +1818,16 @@
         <v>6132324</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>130</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
         <v>5</v>
@@ -1836,10 +1839,10 @@
         <v>43</v>
       </c>
       <c r="I12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K12" t="s">
         <v>31</v>
@@ -1851,7 +1854,7 @@
         <v>29</v>
       </c>
       <c r="N12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O12" t="s">
         <v>90</v>
@@ -1860,22 +1863,22 @@
         <v>91</v>
       </c>
       <c r="Q12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="R12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="T12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="U12" t="s">
         <v>29</v>
       </c>
       <c r="V12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="W12" t="s">
         <v>24</v>
@@ -1889,16 +1892,16 @@
         <v>5928633</v>
       </c>
       <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" t="s">
         <v>81</v>
       </c>
-      <c r="C13" t="s">
-        <v>82</v>
-      </c>
       <c r="D13" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F13" t="s">
         <v>5</v>
@@ -1910,16 +1913,16 @@
         <v>43</v>
       </c>
       <c r="I13" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="J13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="K13" t="s">
         <v>31</v>
       </c>
       <c r="L13" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M13" t="s">
         <v>29</v>
@@ -1934,13 +1937,13 @@
         <v>33</v>
       </c>
       <c r="Q13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R13" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="S13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="T13" t="s">
         <v>29</v>
@@ -1949,7 +1952,7 @@
         <v>29</v>
       </c>
       <c r="V13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="W13" t="s">
         <v>24</v>
@@ -1966,13 +1969,13 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
         <v>5</v>
@@ -1984,10 +1987,10 @@
         <v>43</v>
       </c>
       <c r="I14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="J14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K14" t="s">
         <v>31</v>
@@ -1999,7 +2002,7 @@
         <v>29</v>
       </c>
       <c r="N14" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="O14" t="s">
         <v>90</v>
@@ -2008,13 +2011,13 @@
         <v>91</v>
       </c>
       <c r="Q14" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="R14" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="S14" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="T14" t="s">
         <v>37</v>
@@ -2023,7 +2026,7 @@
         <v>29</v>
       </c>
       <c r="V14" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="W14" t="s">
         <v>24</v>
@@ -2037,58 +2040,58 @@
         <v>3788039</v>
       </c>
       <c r="B15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="F15" t="s">
         <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H15" t="s">
         <v>43</v>
       </c>
       <c r="I15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="J15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="K15" t="s">
         <v>31</v>
       </c>
       <c r="L15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O15" t="s">
         <v>90</v>
       </c>
       <c r="P15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="Q15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="R15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="S15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="T15" t="s">
         <v>29</v>
@@ -2097,7 +2100,7 @@
         <v>29</v>
       </c>
       <c r="V15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="W15" t="s">
         <v>24</v>
@@ -2114,13 +2117,13 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -2132,19 +2135,19 @@
         <v>43</v>
       </c>
       <c r="I16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="K16" t="s">
         <v>110</v>
       </c>
       <c r="L16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M16" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="N16" t="s">
         <v>24</v>
@@ -2162,7 +2165,7 @@
         <v>24</v>
       </c>
       <c r="S16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="T16" t="s">
         <v>29</v>
@@ -2185,16 +2188,16 @@
         <v>3788467</v>
       </c>
       <c r="B17" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C17" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E17" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -2206,37 +2209,37 @@
         <v>43</v>
       </c>
       <c r="I17" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="J17" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="K17" t="s">
         <v>31</v>
       </c>
       <c r="L17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M17" t="s">
         <v>29</v>
       </c>
       <c r="N17" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="O17" t="s">
         <v>29</v>
       </c>
       <c r="P17" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Q17" t="s">
         <v>24</v>
       </c>
       <c r="R17" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="S17" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="T17" t="s">
         <v>29</v>
@@ -2245,7 +2248,7 @@
         <v>29</v>
       </c>
       <c r="V17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="W17" t="s">
         <v>24</v>
@@ -2259,40 +2262,40 @@
         <v>3680804</v>
       </c>
       <c r="B18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C18" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D18" t="s">
         <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H18" t="s">
         <v>43</v>
       </c>
       <c r="I18" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="J18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K18" t="s">
         <v>110</v>
       </c>
       <c r="L18" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="M18" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="N18" t="s">
         <v>24</v>
@@ -2310,7 +2313,7 @@
         <v>24</v>
       </c>
       <c r="S18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="T18" t="s">
         <v>29</v>
@@ -2333,16 +2336,16 @@
         <v>5087863</v>
       </c>
       <c r="B19" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C19" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E19" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -2354,16 +2357,16 @@
         <v>43</v>
       </c>
       <c r="I19" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="J19" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="K19" t="s">
         <v>31</v>
       </c>
       <c r="L19" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="M19" t="s">
         <v>29</v>
@@ -2381,10 +2384,10 @@
         <v>24</v>
       </c>
       <c r="R19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="S19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="T19" t="s">
         <v>29</v>
@@ -2393,7 +2396,7 @@
         <v>29</v>
       </c>
       <c r="V19" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="W19" t="s">
         <v>24</v>

</xml_diff>